<commit_message>
Ajout du script permettant d'automatiser l'insertion des résu dans excel
</commit_message>
<xml_diff>
--- a/database/result_request.xlsx
+++ b/database/result_request.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20070" windowHeight="11513" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20070" windowHeight="11513" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="req1" sheetId="1" r:id="rId1"/>
@@ -388,6 +388,170 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'req13'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>90 25 21 21 10 10 7 6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'req13'!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>plastique</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dechets</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>plastiques</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>sacs</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ocean</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>sac</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>oceans</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'req13'!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>454818</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>92868</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>454818</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>121443</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Graphique 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -862,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1148,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1231,6 +1395,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
commit de merde ça me soule
</commit_message>
<xml_diff>
--- a/database/result_request.xlsx
+++ b/database/result_request.xlsx
@@ -404,10 +404,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -416,22 +412,11 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'req13'!$A$2:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>90 25 21 21 10 10 7 6</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'req13'!$B$2:$B$8</c:f>
+              <c:f>'req11'!$B$2:$B$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>plastique</c:v>
                 </c:pt>
@@ -439,52 +424,55 @@
                   <c:v>dechets</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>ocean</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>plastiques</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>sacs</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>ocean</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>sac</c:v>
+                  <c:v>mer</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>oceans</c:v>
+                  <c:v>etude</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ville</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'req13'!$B$2:$B$9</c:f>
+              <c:f>'req11'!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -506,6 +494,270 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'req12'!$B$2:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>plastique</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dechets</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>plastiques</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>sacs</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ocean</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mer</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>oceans</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>sac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'req12'!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'req13'!$B$2:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>plastique</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dechets</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>plastiques</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>sacs</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ocean</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>sac</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>oceans</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tri</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'req13'!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -523,20 +775,90 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>454818</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>92868</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>564355</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>83344</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>454818</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>121443</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>564355</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>111919</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Graphique 4"/>
+        <xdr:cNvPr id="4" name="Graphique 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>59530</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>59530</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>483393</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>126205</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>483393</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>154780</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -844,7 +1166,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1027,7 +1349,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1133,7 +1455,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1215,6 +1537,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1223,7 +1546,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1305,6 +1628,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1313,7 +1637,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>